<commit_message>
added testng.xml to run tests via maven surefire
</commit_message>
<xml_diff>
--- a/orangeHRM-parameterization-git/src/test/resources/TestData.xlsx
+++ b/orangeHRM-parameterization-git/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W10-Dell\git\orangeHRM-parameterization-git\orangeHRM-parameterization-git\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7AC140-79A8-49B3-AB0D-360EF78A00E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE809FC-EA53-45CA-BBDC-139A31CC30DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>